<commit_message>
added coloring based on selected assessment value
</commit_message>
<xml_diff>
--- a/templates/Gap-Analysis-Template.xlsx
+++ b/templates/Gap-Analysis-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitRepository\git\Consulting.Project.Tools\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB19CAE6-69B8-476C-AFBB-2C5C4741CD4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E6B110-97F0-44D7-8371-893EACCC2B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{38E53BE3-E64D-4BB8-99FF-65D713BF3BF1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{38E53BE3-E64D-4BB8-99FF-65D713BF3BF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>Priority</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>1-N/A</t>
+  </si>
+  <si>
+    <t>Example Requirement…</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,384 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -638,7 +1018,7 @@
   <dimension ref="A2:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,32 +1066,32 @@
         <v>6-Exceeds</v>
       </c>
       <c r="B3" s="17">
-        <f>COUNTIF(Analysis!E$5:E$994,$A3)</f>
-        <v>0</v>
+        <f>COUNTIF(Analysis!E$5:E$995,$A3)</f>
+        <v>1</v>
       </c>
       <c r="C3" s="17">
-        <f>COUNTIF(Analysis!F$5:F$994,$A3)</f>
+        <f>COUNTIF(Analysis!F$5:F$995,$A3)</f>
         <v>0</v>
       </c>
       <c r="D3" s="17">
-        <f>COUNTIF(Analysis!G$5:G$994,$A3)</f>
+        <f>COUNTIF(Analysis!G$5:G$995,$A3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="17">
-        <f>COUNTIF(Analysis!H$5:H$994,$A3)</f>
+        <f>COUNTIF(Analysis!H$5:H$995,$A3)</f>
         <v>0</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="17">
-        <f>COUNTIF(Analysis!J$5:J$994,$A3)</f>
+        <f>COUNTIF(Analysis!J$5:J$995,$A3)</f>
         <v>0</v>
       </c>
       <c r="H3" s="17">
-        <f>COUNTIF(Analysis!K$5:K$994,$A3)</f>
+        <f>COUNTIF(Analysis!K$5:K$995,$A3)</f>
         <v>0</v>
       </c>
       <c r="I3" s="17">
-        <f>COUNTIF(Analysis!L$5:L$994,$A3)</f>
+        <f>COUNTIF(Analysis!L$5:L$995,$A3)</f>
         <v>0</v>
       </c>
     </row>
@@ -721,32 +1101,32 @@
         <v>5-Meets</v>
       </c>
       <c r="B4" s="17">
-        <f>COUNTIF(Analysis!E$5:E$994,$A4)</f>
-        <v>0</v>
+        <f>COUNTIF(Analysis!E$5:E$995,$A4)</f>
+        <v>1</v>
       </c>
       <c r="C4" s="17">
-        <f>COUNTIF(Analysis!F$5:F$994,$A4)</f>
+        <f>COUNTIF(Analysis!F$5:F$995,$A4)</f>
         <v>0</v>
       </c>
       <c r="D4" s="17">
-        <f>COUNTIF(Analysis!G$5:G$994,$A4)</f>
+        <f>COUNTIF(Analysis!G$5:G$995,$A4)</f>
         <v>0</v>
       </c>
       <c r="E4" s="17">
-        <f>COUNTIF(Analysis!H$5:H$994,$A4)</f>
+        <f>COUNTIF(Analysis!H$5:H$995,$A4)</f>
         <v>0</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="17">
-        <f>COUNTIF(Analysis!J$5:J$994,$A4)</f>
+        <f>COUNTIF(Analysis!J$5:J$995,$A4)</f>
         <v>0</v>
       </c>
       <c r="H4" s="17">
-        <f>COUNTIF(Analysis!K$5:K$994,$A4)</f>
+        <f>COUNTIF(Analysis!K$5:K$995,$A4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="17">
-        <f>COUNTIF(Analysis!L$5:L$994,$A4)</f>
+        <f>COUNTIF(Analysis!L$5:L$995,$A4)</f>
         <v>0</v>
       </c>
     </row>
@@ -756,32 +1136,32 @@
         <v>4-Partial</v>
       </c>
       <c r="B5" s="17">
-        <f>COUNTIF(Analysis!E$5:E$994,$A5)</f>
-        <v>0</v>
+        <f>COUNTIF(Analysis!E$5:E$995,$A5)</f>
+        <v>1</v>
       </c>
       <c r="C5" s="17">
-        <f>COUNTIF(Analysis!F$5:F$994,$A5)</f>
+        <f>COUNTIF(Analysis!F$5:F$995,$A5)</f>
         <v>0</v>
       </c>
       <c r="D5" s="17">
-        <f>COUNTIF(Analysis!G$5:G$994,$A5)</f>
+        <f>COUNTIF(Analysis!G$5:G$995,$A5)</f>
         <v>0</v>
       </c>
       <c r="E5" s="17">
-        <f>COUNTIF(Analysis!H$5:H$994,$A5)</f>
+        <f>COUNTIF(Analysis!H$5:H$995,$A5)</f>
         <v>0</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="17">
-        <f>COUNTIF(Analysis!J$5:J$994,$A5)</f>
+        <f>COUNTIF(Analysis!J$5:J$995,$A5)</f>
         <v>0</v>
       </c>
       <c r="H5" s="17">
-        <f>COUNTIF(Analysis!K$5:K$994,$A5)</f>
+        <f>COUNTIF(Analysis!K$5:K$995,$A5)</f>
         <v>0</v>
       </c>
       <c r="I5" s="17">
-        <f>COUNTIF(Analysis!L$5:L$994,$A5)</f>
+        <f>COUNTIF(Analysis!L$5:L$995,$A5)</f>
         <v>0</v>
       </c>
     </row>
@@ -791,32 +1171,32 @@
         <v>3-Roadmap</v>
       </c>
       <c r="B6" s="17">
-        <f>COUNTIF(Analysis!E$5:E$994,$A6)</f>
-        <v>0</v>
+        <f>COUNTIF(Analysis!E$5:E$995,$A6)</f>
+        <v>1</v>
       </c>
       <c r="C6" s="17">
-        <f>COUNTIF(Analysis!F$5:F$994,$A6)</f>
+        <f>COUNTIF(Analysis!F$5:F$995,$A6)</f>
         <v>0</v>
       </c>
       <c r="D6" s="17">
-        <f>COUNTIF(Analysis!G$5:G$994,$A6)</f>
+        <f>COUNTIF(Analysis!G$5:G$995,$A6)</f>
         <v>0</v>
       </c>
       <c r="E6" s="17">
-        <f>COUNTIF(Analysis!H$5:H$994,$A6)</f>
+        <f>COUNTIF(Analysis!H$5:H$995,$A6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="17">
-        <f>COUNTIF(Analysis!J$5:J$994,$A6)</f>
+        <f>COUNTIF(Analysis!J$5:J$995,$A6)</f>
         <v>0</v>
       </c>
       <c r="H6" s="17">
-        <f>COUNTIF(Analysis!K$5:K$994,$A6)</f>
+        <f>COUNTIF(Analysis!K$5:K$995,$A6)</f>
         <v>0</v>
       </c>
       <c r="I6" s="17">
-        <f>COUNTIF(Analysis!L$5:L$994,$A6)</f>
+        <f>COUNTIF(Analysis!L$5:L$995,$A6)</f>
         <v>0</v>
       </c>
     </row>
@@ -826,32 +1206,32 @@
         <v>2-Gap</v>
       </c>
       <c r="B7" s="17">
-        <f>COUNTIF(Analysis!E$5:E$994,$A7)</f>
-        <v>0</v>
+        <f>COUNTIF(Analysis!E$5:E$995,$A7)</f>
+        <v>1</v>
       </c>
       <c r="C7" s="17">
-        <f>COUNTIF(Analysis!F$5:F$994,$A7)</f>
+        <f>COUNTIF(Analysis!F$5:F$995,$A7)</f>
         <v>0</v>
       </c>
       <c r="D7" s="17">
-        <f>COUNTIF(Analysis!G$5:G$994,$A7)</f>
+        <f>COUNTIF(Analysis!G$5:G$995,$A7)</f>
         <v>0</v>
       </c>
       <c r="E7" s="17">
-        <f>COUNTIF(Analysis!H$5:H$994,$A7)</f>
+        <f>COUNTIF(Analysis!H$5:H$995,$A7)</f>
         <v>0</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="17">
-        <f>COUNTIF(Analysis!J$5:J$994,$A7)</f>
+        <f>COUNTIF(Analysis!J$5:J$995,$A7)</f>
         <v>0</v>
       </c>
       <c r="H7" s="17">
-        <f>COUNTIF(Analysis!K$5:K$994,$A7)</f>
+        <f>COUNTIF(Analysis!K$5:K$995,$A7)</f>
         <v>0</v>
       </c>
       <c r="I7" s="17">
-        <f>COUNTIF(Analysis!L$5:L$994,$A7)</f>
+        <f>COUNTIF(Analysis!L$5:L$995,$A7)</f>
         <v>0</v>
       </c>
     </row>
@@ -861,32 +1241,32 @@
         <v>1-N/A</v>
       </c>
       <c r="B8" s="17">
-        <f>COUNTIF(Analysis!E$5:E$994,$A8)</f>
-        <v>0</v>
+        <f>COUNTIF(Analysis!E$5:E$995,$A8)</f>
+        <v>1</v>
       </c>
       <c r="C8" s="17">
-        <f>COUNTIF(Analysis!F$5:F$994,$A8)</f>
+        <f>COUNTIF(Analysis!F$5:F$995,$A8)</f>
         <v>0</v>
       </c>
       <c r="D8" s="17">
-        <f>COUNTIF(Analysis!G$5:G$994,$A8)</f>
+        <f>COUNTIF(Analysis!G$5:G$995,$A8)</f>
         <v>0</v>
       </c>
       <c r="E8" s="17">
-        <f>COUNTIF(Analysis!H$5:H$994,$A8)</f>
+        <f>COUNTIF(Analysis!H$5:H$995,$A8)</f>
         <v>0</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="17">
-        <f>COUNTIF(Analysis!J$5:J$994,$A8)</f>
+        <f>COUNTIF(Analysis!J$5:J$995,$A8)</f>
         <v>0</v>
       </c>
       <c r="H8" s="17">
-        <f>COUNTIF(Analysis!K$5:K$994,$A8)</f>
+        <f>COUNTIF(Analysis!K$5:K$995,$A8)</f>
         <v>0</v>
       </c>
       <c r="I8" s="17">
-        <f>COUNTIF(Analysis!L$5:L$994,$A8)</f>
+        <f>COUNTIF(Analysis!L$5:L$995,$A8)</f>
         <v>0</v>
       </c>
     </row>
@@ -897,11 +1277,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA968C0-781F-4DA5-AD51-12B2BD647FF9}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,6 +1425,15 @@
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
@@ -1053,6 +1442,15 @@
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
@@ -1061,6 +1459,15 @@
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -1069,36 +1476,71 @@
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>1.05</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
-        <v>2.02</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>16</v>
@@ -1106,7 +1548,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
-        <v>2.0299999999999998</v>
+        <v>2.02</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>16</v>
@@ -1114,41 +1556,41 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
-        <v>2.04</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>2.04</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
         <v>3</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
-        <v>3.01</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
-        <v>3.02</v>
+        <v>3.01</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>17</v>
@@ -1156,7 +1598,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
-        <v>3.03</v>
+        <v>3.02</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>17</v>
@@ -1164,41 +1606,41 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
-        <v>3.04</v>
+        <v>3.03</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>3.04</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
         <v>4</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="8">
-        <v>4.01</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
-        <v>4.0199999999999996</v>
+        <v>4.01</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>18</v>
@@ -1206,7 +1648,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
-        <v>4.03</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>18</v>
@@ -1220,22 +1662,118 @@
         <v>18</v>
       </c>
     </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>4.03</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{011C9516-A7B1-4265-B228-7F99A1E865B0}">
+            <xm:f>Lookups!$B$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{73EDEF68-CEE6-4385-9A71-4B4DA6E8A833}">
+            <xm:f>Lookups!$B$5</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{E4E9C934-A2DF-4B24-B6E1-A49CD9DBF45C}">
+            <xm:f>Lookups!$B$4</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C5700"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFFF00"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{29751344-8A6E-40F5-87F3-6536CFB5A106}">
+            <xm:f>Lookups!$B$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.79998168889431442"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{7796F7D2-C3BD-4779-95A2-02A6542C9617}">
+            <xm:f>Lookups!$B$2</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{6AC49287-7D18-4AF1-85AC-71C6E075B746}">
+            <xm:f>Lookups!$B$7</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0" tint="-0.499984740745262"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E1:L1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DCD886CE-70A5-4A9A-8206-FEFEDDDE312A}">
           <x14:formula1>
             <xm:f>Lookups!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>J6:L934 E6:H1747</xm:sqref>
+          <xm:sqref>J6:L935 E6:H1748</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D3CE57C3-11EF-424C-9CE8-92BFF5315A31}">
           <x14:formula1>
             <xm:f>Lookups!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C6:C934</xm:sqref>
+          <xm:sqref>C6:C935</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1370,8 +1908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8F8C79-E982-4260-BD01-B6774CEA507F}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>